<commit_message>
Fixed bugs and more improvements
</commit_message>
<xml_diff>
--- a/2017_gains (13)_edited.xlsx
+++ b/2017_gains (13)_edited.xlsx
@@ -544,7 +544,7 @@
         <v>13</v>
       </c>
       <c r="F3">
-        <v>99738.98000000001</v>
+        <v>99648.61</v>
       </c>
     </row>
     <row r="4" spans="1:18">
@@ -555,7 +555,7 @@
         <v>14</v>
       </c>
       <c r="F4">
-        <v>1638.864778200019</v>
+        <v>1633.801242200003</v>
       </c>
     </row>
     <row r="5" spans="1:18">
@@ -563,7 +563,7 @@
         <v>10</v>
       </c>
       <c r="F5">
-        <v>98100.11522179999</v>
+        <v>98014.8087578</v>
       </c>
     </row>
     <row r="6" spans="1:18">
@@ -585,7 +585,7 @@
         <v>16</v>
       </c>
       <c r="F7">
-        <v>98100.11522179999</v>
+        <v>98014.8087578</v>
       </c>
     </row>
     <row r="13" spans="1:18">
@@ -717,10 +717,10 @@
         <v>42777</v>
       </c>
       <c r="F15">
-        <v>382.4307379785647</v>
+        <v>381.0163426460692</v>
       </c>
       <c r="G15">
-        <v>24274.68564353738</v>
+        <v>24184.90728980595</v>
       </c>
       <c r="H15">
         <v>33477170.5116954</v>
@@ -729,25 +729,25 @@
         <v>33535878.4762692</v>
       </c>
       <c r="J15">
-        <v>4854.95</v>
+        <v>4837</v>
       </c>
       <c r="K15">
-        <v>76.48999999999999</v>
+        <v>76.2</v>
       </c>
       <c r="L15">
-        <v>0.1338574999999906</v>
+        <v>0.133349999999993</v>
       </c>
       <c r="M15">
-        <v>76.62385749999999</v>
+        <v>76.33335</v>
       </c>
       <c r="N15">
-        <v>4778.46</v>
+        <v>4760.8</v>
       </c>
       <c r="O15">
-        <v>4778.3261425</v>
+        <v>4760.66665</v>
       </c>
       <c r="P15">
-        <v>4778.3261425</v>
+        <v>4760.66665</v>
       </c>
       <c r="Q15" t="s">
         <v>20</v>
@@ -773,10 +773,10 @@
         <v>42884</v>
       </c>
       <c r="F16">
-        <v>382.284929356358</v>
+        <v>380.8710732876146</v>
       </c>
       <c r="G16">
-        <v>8243.274725274727</v>
+        <v>8212.787507229612</v>
       </c>
       <c r="H16">
         <v>33477170.5116954</v>
@@ -785,25 +785,25 @@
         <v>33838306.2380792</v>
       </c>
       <c r="J16">
-        <v>9976.84</v>
+        <v>9939.940000000001</v>
       </c>
       <c r="K16">
-        <v>462.68</v>
+        <v>460.97</v>
       </c>
       <c r="L16">
-        <v>4.992317200000059</v>
+        <v>4.973866300000054</v>
       </c>
       <c r="M16">
-        <v>467.6723172000001</v>
+        <v>465.9438663000001</v>
       </c>
       <c r="N16">
-        <v>9514.16</v>
+        <v>9478.970000000001</v>
       </c>
       <c r="O16">
-        <v>9509.1676828</v>
+        <v>9473.9961337</v>
       </c>
       <c r="P16">
-        <v>9509.1676828</v>
+        <v>9473.9961337</v>
       </c>
       <c r="Q16" t="s">
         <v>20</v>
@@ -829,10 +829,10 @@
         <v>42924</v>
       </c>
       <c r="F17">
-        <v>382.2757777777778</v>
+        <v>380.8619555555555</v>
       </c>
       <c r="G17">
-        <v>10671.14944444445</v>
+        <v>10631.68288888889</v>
       </c>
       <c r="H17">
         <v>33477170.5116954</v>
@@ -841,25 +841,25 @@
         <v>33569481.5609147</v>
       </c>
       <c r="J17">
-        <v>9604.030000000001</v>
+        <v>9568.51</v>
       </c>
       <c r="K17">
-        <v>344.05</v>
+        <v>342.78</v>
       </c>
       <c r="L17">
-        <v>0.9495780000000309</v>
+        <v>0.9460728000000245</v>
       </c>
       <c r="M17">
-        <v>344.999578</v>
+        <v>343.7260728</v>
       </c>
       <c r="N17">
-        <v>9259.980000000001</v>
+        <v>9225.73</v>
       </c>
       <c r="O17">
-        <v>9259.030422</v>
+        <v>9224.7839272</v>
       </c>
       <c r="P17">
-        <v>9259.030422</v>
+        <v>9224.7839272</v>
       </c>
       <c r="Q17" t="s">
         <v>20</v>
@@ -885,7 +885,7 @@
         <v>43038</v>
       </c>
       <c r="F18">
-        <v>382.25625</v>
+        <v>383.67</v>
       </c>
       <c r="G18">
         <v>21680.9712</v>
@@ -900,22 +900,22 @@
         <v>4336.19</v>
       </c>
       <c r="K18">
-        <v>76.45</v>
+        <v>76.73</v>
       </c>
       <c r="L18">
-        <v>0.7476809999999858</v>
+        <v>0.7504193999999984</v>
       </c>
       <c r="M18">
-        <v>77.19768099999999</v>
+        <v>77.4804194</v>
       </c>
       <c r="N18">
-        <v>4259.74</v>
+        <v>4259.46</v>
       </c>
       <c r="O18">
-        <v>4258.992319</v>
+        <v>4258.7095806</v>
       </c>
       <c r="P18">
-        <v>4258.992319</v>
+        <v>4258.7095806</v>
       </c>
       <c r="Q18" t="s">
         <v>20</v>
@@ -941,7 +941,7 @@
         <v>43059</v>
       </c>
       <c r="F19">
-        <v>382.3079411764705</v>
+        <v>382.4167058823529</v>
       </c>
       <c r="G19">
         <v>28937.71411764706</v>
@@ -956,22 +956,22 @@
         <v>4919.41</v>
       </c>
       <c r="K19">
-        <v>64.98999999999999</v>
+        <v>65.01000000000001</v>
       </c>
       <c r="L19">
-        <v>0.4399822999999969</v>
+        <v>0.4401177000000018</v>
       </c>
       <c r="M19">
-        <v>65.42998229999999</v>
+        <v>65.45011770000001</v>
       </c>
       <c r="N19">
-        <v>4854.42</v>
+        <v>4854.4</v>
       </c>
       <c r="O19">
-        <v>4853.9800177</v>
+        <v>4853.9598823</v>
       </c>
       <c r="P19">
-        <v>4853.9800177</v>
+        <v>4853.9598823</v>
       </c>
       <c r="Q19" t="s">
         <v>20</v>
@@ -997,7 +997,7 @@
         <v>43067</v>
       </c>
       <c r="F20">
-        <v>382.2817616405649</v>
+        <v>380.9766745453482</v>
       </c>
       <c r="G20">
         <v>35538.38650545067</v>
@@ -1012,22 +1012,22 @@
         <v>56043.97</v>
       </c>
       <c r="K20">
-        <v>602.86</v>
+        <v>600.8</v>
       </c>
       <c r="L20">
-        <v>4.081362199999944</v>
+        <v>4.06741599999998</v>
       </c>
       <c r="M20">
-        <v>606.9413622</v>
+        <v>604.8674159999999</v>
       </c>
       <c r="N20">
-        <v>55441.11</v>
+        <v>55443.17</v>
       </c>
       <c r="O20">
-        <v>55437.0286378</v>
+        <v>55439.102584</v>
       </c>
       <c r="P20">
-        <v>55437.0286378</v>
+        <v>55439.102584</v>
       </c>
       <c r="Q20" t="s">
         <v>20</v>

</xml_diff>